<commit_message>
Added examples + Minor changes
</commit_message>
<xml_diff>
--- a/Dictionaries/CSPCore/Examples/example_minimal_excel.xlsx
+++ b/Dictionaries/CSPCore/Examples/example_minimal_excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nfrancia\Desktop\Projects\CSPDataStandards\COMCIFS_Structure_Prediction_Dictionary\Dictionaries\CSPCore\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22AD56F-6B17-49DE-AEC7-C22ADF7B7689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95B6C82-4AA5-4E09-A897-BAEC7C8D6399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -825,7 +825,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.7109375" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Examples and minor corrections
</commit_message>
<xml_diff>
--- a/Dictionaries/CSPCore/Examples/example_minimal_excel.xlsx
+++ b/Dictionaries/CSPCore/Examples/example_minimal_excel.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nfrancia\Desktop\Projects\CSPDataStandards\COMCIFS_Structure_Prediction_Dictionary\Dictionaries\CSPCore\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95B6C82-4AA5-4E09-A897-BAEC7C8D6399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B30D4693-91C1-4B21-B01D-B3D069AD0A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -214,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -260,17 +261,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -435,30 +425,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -467,79 +460,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -825,7 +824,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D12" sqref="B5:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="45.7109375" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -863,152 +862,152 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="9" t="s">
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="27"/>
+      <c r="B13" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="15" t="s">
+      <c r="A14" s="28"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="19" t="s">
+      <c r="A16" s="30"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="9" t="s">
+      <c r="A17" s="30"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="21" t="s">
+      <c r="A18" s="31"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="17" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>